<commit_message>
# Avance con la presentacion final
</commit_message>
<xml_diff>
--- a/presentations/CostosReal.xlsx
+++ b/presentations/CostosReal.xlsx
@@ -16,12 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Hs Planificadas Totales</t>
-  </si>
-  <si>
-    <t>Hs Planificadas Completadas</t>
-  </si>
-  <si>
     <t>Hs Reales Utilizadas</t>
   </si>
   <si>
@@ -29,6 +23,12 @@
   </si>
   <si>
     <t>Costos</t>
+  </si>
+  <si>
+    <t>Hs Completadas</t>
+  </si>
+  <si>
+    <t>Hs Planificadas</t>
   </si>
 </sst>
 </file>
@@ -180,7 +180,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hs Planificadas Totales</c:v>
+                  <c:v>Hs Planificadas</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -243,7 +243,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hs Planificadas Completadas</c:v>
+                  <c:v>Hs Completadas</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -361,11 +361,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="105254272"/>
+        <c:axId val="105319808"/>
         <c:axId val="106579840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105254272"/>
+        <c:axId val="105319808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,7 +445,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105254272"/>
+        <c:crossAx val="105319808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -483,7 +483,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -529,8 +529,8 @@
   <autoFilter ref="A2:D7"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Sprint / Horas" dataDxfId="3"/>
-    <tableColumn id="2" name="Hs Planificadas Totales" dataDxfId="2"/>
-    <tableColumn id="3" name="Hs Planificadas Completadas" dataDxfId="1"/>
+    <tableColumn id="2" name="Hs Planificadas" dataDxfId="2"/>
+    <tableColumn id="3" name="Hs Completadas" dataDxfId="1"/>
     <tableColumn id="4" name="Hs Reales Utilizadas" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -825,7 +825,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -839,23 +839,23 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>